<commit_message>
Upgraded to python 3.12. Tested pickaxe run, process pickaxe (though not thermo calcs), path viewer. Installed equilibrator-assets, upgraded pint to resolve issue with frozen dataclass inheriting non-frozen dataclass. Added issue tracking csv
</commit_message>
<xml_diff>
--- a/artifacts/241021_biocasp_issues.xlsx
+++ b/artifacts/241021_biocasp_issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\stef\bottle\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE2A26C-0739-43AF-BA70-35FFD33AEB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564F0E4A-18BC-4548-AC2D-A20F80AD49AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Issue</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>Add ability to save specific paths of interest from the path viewer</t>
+  </si>
+  <si>
+    <t>Update expansion processing tracking to have a column each for rcmcs_processed, thermo_processed</t>
+  </si>
+  <si>
+    <t>Change logic of process all to accommodate this</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Posted to GH</t>
   </si>
 </sst>
 </file>
@@ -246,31 +258,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color theme="0"/>
@@ -292,20 +280,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -590,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +576,10 @@
     <col min="3" max="3" width="47.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="66.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -621,8 +595,11 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -638,8 +615,11 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -655,8 +635,11 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -673,7 +656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -687,7 +670,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -695,7 +678,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -712,7 +695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -729,7 +712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -746,7 +729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -763,7 +746,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -774,12 +757,22 @@
         <v>34</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E10" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
-      <sortCondition ref="B1:B10"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:F12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
     <sortCondition ref="B2:B9"/>
   </sortState>
@@ -796,13 +789,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed issue with poetry not installing my fork of minedatabase. Slight update to pickaxe pickling method. Tested up to thermo and image generation the post_processing of a forward reverse combo case. Added ability to process these by reversing reverse expansion reactions.
</commit_message>
<xml_diff>
--- a/artifacts/241021_biocasp_issues.xlsx
+++ b/artifacts/241021_biocasp_issues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\stef\bottle\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564F0E4A-18BC-4548-AC2D-A20F80AD49AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E080577-4154-471A-9227-18300564D85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Issue</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Posted to GH</t>
+  </si>
+  <si>
+    <t>Update reaction hashing to be stoich sensitive</t>
+  </si>
+  <si>
+    <t>Expansions and Post-processing</t>
   </si>
 </sst>
 </file>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,6 +775,17 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue with template alignment reaction to rule that was resulting in minified rules apparently not recapitulating imt rules
</commit_message>
<xml_diff>
--- a/artifacts/241021_biocasp_issues.xlsx
+++ b/artifacts/241021_biocasp_issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\stef\bottle\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E080577-4154-471A-9227-18300564D85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F6D4FD-EAE9-4447-BC4C-D8FE17EC47FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Issue</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Expansions and Post-processing</t>
+  </si>
+  <si>
+    <t>Resoved by SP</t>
+  </si>
+  <si>
+    <t>Return predicted reactions in order of rule that generated them</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,6 +723,9 @@
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -786,6 +795,17 @@
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>